<commit_message>
add-expiration-date.py ready for verification
</commit_message>
<xml_diff>
--- a/Barcodes.xlsx
+++ b/Barcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lander Wuyts\IT\Sys Eng Projectweek\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC79D9F5-1922-42C0-ABD8-F477AFC8075A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F407F7AF-3F68-4179-9F5D-433303F81667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5239CB96-FA84-43C4-98A1-2144099ABCCF}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -93,10 +94,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,16 +417,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16.88671875" style="4" customWidth="1"/>
     <col min="3" max="3" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -434,8 +438,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>40833666</v>
+      <c r="A2" s="4">
+        <v>7610700949085</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -445,8 +449,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>123</v>
+      <c r="A3" s="4">
+        <v>5414150631147</v>
       </c>
       <c r="B3">
         <v>5</v>

</xml_diff>

<commit_message>
document script without propper layout
</commit_message>
<xml_diff>
--- a/Barcodes.xlsx
+++ b/Barcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lander Wuyts\IT\Sys Eng Projectweek\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3B3AFA-3413-4DDF-8F2D-3190BD989601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99ED55C-32EA-4E2B-855F-55471075B018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5239CB96-FA84-43C4-98A1-2144099ABCCF}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Document script ready for verification
</commit_message>
<xml_diff>
--- a/Barcodes.xlsx
+++ b/Barcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lander Wuyts\IT\Sys Eng Projectweek\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99ED55C-32EA-4E2B-855F-55471075B018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCAAF57-5DE1-4D4D-A153-03F49CD36F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5239CB96-FA84-43C4-98A1-2144099ABCCF}"/>
   </bookViews>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8315AB79-82FD-4F9F-8156-629013D4B21E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,6 +469,50 @@
         <v>44593</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>3502110008091</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44776</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5410013110002</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>5411028070480</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44590</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>5411188115472</v>
+      </c>
+      <c r="B8">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44589</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>